<commit_message>
updates to court case query results mapping spreadsheet
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Query_Results/artifacts/service_model/information_model/IEPD/documentation/Court_Case_Query_Results-Mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="1171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="1170">
   <si>
     <t>Race</t>
   </si>
@@ -3502,18 +3502,9 @@
     <t>ccq-res-doc:CourtCaseQueryResults/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargePlea/j:PleaDescriptionText</t>
   </si>
   <si>
-    <t>ccq-res-doc:CourtCaseQueryResults/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargePlea/j:PleaRecommendationjText</t>
-  </si>
-  <si>
     <t>ccq-res-doc:CourtCaseQueryResults/nc:Vehicle/j:ConveyanceAugmentation/j:ModelYearRange/nc:StartDate/nc:YearDate</t>
   </si>
   <si>
-    <t>ccq-res-doc:CourtCaseQueryResults/nc:Vehicle/nc:VehicleIdentification/intel:IdentificationAugmentation/intel:IdentificationIssuingLocalityText</t>
-  </si>
-  <si>
-    <t>ccq-res-doc:CourtCaseQueryResults/nc:Vehicle/nc:VehicleIdentification/intel:IdentificationAugmentation/intel:IdentificationIssuingStateName</t>
-  </si>
-  <si>
     <t>ccq-res-doc:CourtCaseQueryResults/nc:Vehicle/nc:ItemColor/j:ConveyanceColorPrimaryCode</t>
   </si>
   <si>
@@ -3536,13 +3527,19 @@
   </si>
   <si>
     <t>ccq-res-doc:CourtCaseQueryResults/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargeSentence/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>ccq-res-doc:CourtCaseQueryResults/nc:Case/j:CaseAugmentation/j:CaseCharge/j:ChargePlea/j:PleaRecommendationText</t>
+  </si>
+  <si>
+    <t>ccq-res-doc:CourtCaseQueryResults/nc:Vehicle/nc:VehicleIdentification/j:ConveyanceRegistrationPlateIdentification/nc:IdentificationID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3640,6 +3637,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -3713,7 +3717,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="785">
+  <cellStyleXfs count="789">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4499,8 +4503,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -4670,8 +4678,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="154" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="785">
+  <cellStyles count="789">
     <cellStyle name="Calculation" xfId="154" builtinId="22"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -5064,6 +5081,8 @@
     <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -5455,6 +5474,8 @@
     <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5788,8 +5809,8 @@
   <dimension ref="A1:J289"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="2" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -8528,7 +8549,7 @@
         <v>663</v>
       </c>
       <c r="C129" s="23"/>
-      <c r="D129" s="23" t="s">
+      <c r="D129" s="59" t="s">
         <v>1127</v>
       </c>
       <c r="E129" s="23" t="s">
@@ -9505,7 +9526,7 @@
         <v>751</v>
       </c>
       <c r="D175" s="28" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="E175" s="3" t="s">
         <v>11</v>
@@ -9528,7 +9549,7 @@
         <v>752</v>
       </c>
       <c r="D176" s="28" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>11</v>
@@ -9953,15 +9974,15 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="42">
-      <c r="A197" s="32" t="s">
+      <c r="A197" s="61" t="s">
         <v>311</v>
       </c>
       <c r="B197" s="10" t="s">
         <v>313</v>
       </c>
       <c r="C197" s="26"/>
-      <c r="D197" s="26" t="s">
-        <v>1159</v>
+      <c r="D197" s="60" t="s">
+        <v>1168</v>
       </c>
       <c r="E197" s="3" t="s">
         <v>566</v>
@@ -9983,7 +10004,7 @@
       <c r="C198" s="26" t="s">
         <v>1058</v>
       </c>
-      <c r="D198" s="26" t="s">
+      <c r="D198" s="60" t="s">
         <v>1158</v>
       </c>
       <c r="E198" s="3" t="s">
@@ -10560,7 +10581,7 @@
       </c>
       <c r="C227" s="10"/>
       <c r="D227" s="10" t="s">
-        <v>1161</v>
+        <v>1169</v>
       </c>
       <c r="E227" s="3" t="s">
         <v>828</v>
@@ -10581,7 +10602,7 @@
       </c>
       <c r="C228" s="10"/>
       <c r="D228" s="10" t="s">
-        <v>1162</v>
+        <v>1169</v>
       </c>
       <c r="E228" s="3" t="s">
         <v>828</v>
@@ -10673,7 +10694,7 @@
         <v>827</v>
       </c>
       <c r="D232" s="10" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="E232" s="3" t="s">
         <v>828</v>
@@ -10694,7 +10715,7 @@
       </c>
       <c r="C233" s="10"/>
       <c r="D233" s="10" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="E233" s="3" t="s">
         <v>828</v>
@@ -11108,7 +11129,7 @@
       </c>
       <c r="C260" s="10"/>
       <c r="D260" s="32" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="E260" s="3" t="s">
         <v>847</v>
@@ -11152,7 +11173,7 @@
       </c>
       <c r="C262" s="10"/>
       <c r="D262" s="32" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="E262" s="3" t="s">
         <v>847</v>
@@ -11301,7 +11322,7 @@
       </c>
       <c r="C269" s="28"/>
       <c r="D269" s="28" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="E269" s="20" t="s">
         <v>872</v>
@@ -11322,7 +11343,7 @@
       </c>
       <c r="C270" s="32"/>
       <c r="D270" s="28" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="E270" s="3" t="s">
         <v>872</v>
@@ -11343,7 +11364,7 @@
       </c>
       <c r="C271" s="28"/>
       <c r="D271" s="28" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="E271" s="20" t="s">
         <v>872</v>

</xml_diff>